<commit_message>
prep_01 working on formatting UI
</commit_message>
<xml_diff>
--- a/excel_source/sales_data_copy.xlsx
+++ b/excel_source/sales_data_copy.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/suryaganesan/vscode/ml/projects/reporter/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/suryaganesan/vscode/ml/projects/reporter/excel_source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDE65AFF-6B70-C847-8FF4-45AD0DEC0A1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A56A8B62-424C-A945-8FC9-9FB6C11AB030}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="520" windowWidth="28800" windowHeight="16620" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1059,8 +1059,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -1106,11 +1114,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1415,8 +1424,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V10407"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1427,71 +1436,71 @@
     <col min="14" max="14" width="29.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="Q1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="R1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
+      <c r="S1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="T1" t="s">
+      <c r="T1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="U1" t="s">
+      <c r="U1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="V1" t="s">
+      <c r="V1" s="4" t="s">
         <v>21</v>
       </c>
     </row>
@@ -7958,7 +7967,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>

</xml_diff>